<commit_message>
Update Tabelas Banco de dados.xlsx
</commit_message>
<xml_diff>
--- a/Documentação/Tabelas Banco de dados.xlsx
+++ b/Documentação/Tabelas Banco de dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsadm\Desktop\Projeto-Integrador4_DeskOps\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E973A01-B594-4677-BDD9-9411975E9EE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D22F0A2-C559-4743-9F21-6A68B9FB7678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{FFEF2987-F367-4794-9A99-EFB20DF468E5}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Restrição</t>
   </si>
   <si>
-    <t>Tabela: Usuarios(Users)</t>
-  </si>
-  <si>
     <t>Tabela: Ambientes(Envirmonmet)</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>creation_date</t>
+  </si>
+  <si>
+    <t>Tabela: Usuarios(CustomUsers)</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C240059-42CC-43FC-9ED0-9159EF99736A}">
   <dimension ref="B2:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +677,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -768,7 +768,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -787,7 +787,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
@@ -814,20 +814,20 @@
         <v>6</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>11</v>
@@ -878,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>16</v>
@@ -889,7 +889,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>16</v>
@@ -898,61 +898,61 @@
     </row>
     <row r="27" spans="2:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -975,7 +975,7 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
@@ -985,15 +985,15 @@
         <v>9</v>
       </c>
       <c r="C36" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>11</v>
@@ -1018,44 +1018,44 @@
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="D41" s="14"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
@@ -1065,7 +1065,7 @@
         <v>9</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>21</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
@@ -1098,18 +1098,18 @@
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>16</v>
@@ -1117,18 +1117,18 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="21"/>
@@ -1138,7 +1138,7 @@
         <v>9</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>21</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
@@ -1157,21 +1157,21 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>16</v>
@@ -1179,24 +1179,24 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>